<commit_message>
Orchestrator queue replaced by a string list.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathAdvancedCourse\PerformerHashes\PerformerHashes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CF5B8C-0057-4D6E-BF51-B41257B8DA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53086E8-4637-4EEF-93E1-178B9FB99752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>UiPath</t>
   </si>
   <si>
-    <t>Data\Output\UiPathHashesVr2.xlsx</t>
+    <t>Data\Output\UiPathHashesVr3.xlsx</t>
   </si>
 </sst>
 </file>

</xml_diff>